<commit_message>
Added Paper 15 of Hosny
</commit_message>
<xml_diff>
--- a/Papers/Papers.xlsx
+++ b/Papers/Papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation-Project\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18690C84-76C9-4C37-AA3F-D1A23F57538D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FAC97C-9A12-4C48-82C2-47DFD554E784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>6. IIHT: Medical Report Generation with
 Image-to-Indicator Hierarchical Transformer.pdf</t>
@@ -417,9 +417,6 @@
     <t>MIMIC_CXR</t>
   </si>
   <si>
-    <t>Highly Recommneded</t>
-  </si>
-  <si>
     <t>Hosny</t>
   </si>
   <si>
@@ -427,14 +424,6 @@
   </si>
   <si>
     <t>5. Generating Radiology Reports via Memory-driven Transformer.pdf</t>
-  </si>
-  <si>
-    <t>1. the visual extractor
-2. the encoder
-3. the decoder, where the proposed memory and the integration of the memory into Transformer are mainly performed in the decoder</t>
-  </si>
-  <si>
-    <t>generate large text but it's end to end</t>
   </si>
   <si>
     <t>RG-L</t>
@@ -548,6 +537,31 @@
   </si>
   <si>
     <t>reasoning</t>
+  </si>
+  <si>
+    <t>Highly Recommneded
+Good Architecture</t>
+  </si>
+  <si>
+    <t>1. the visual extractor (Pretrianed)
+2. the encoder
+3. the decoder, where the proposed memory and the integration of the memory into Transformer are mainly performed in the decoder</t>
+  </si>
+  <si>
+    <t>generate large text but it's end to end
+Memory [Decoder larger history]</t>
+  </si>
+  <si>
+    <t>Hosy</t>
+  </si>
+  <si>
+    <t>CNN+RNN + Reniformect learning Learning</t>
+  </si>
+  <si>
+    <t>15.Clinically Accurate Chest X-Ray Report Generation.pdf</t>
+  </si>
+  <si>
+    <t>multi_model</t>
   </si>
 </sst>
 </file>
@@ -853,53 +867,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1234,8 +1248,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N248"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1257,73 +1271,77 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>84</v>
+      <c r="C2" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="44"/>
-      <c r="C3" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="46" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="37" t="s">
         <v>38</v>
       </c>
+      <c r="F3" s="37"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32" t="s">
+      <c r="A5" s="41"/>
+      <c r="B5" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32" t="s">
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="41" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="7" t="s">
         <v>49</v>
       </c>
@@ -1333,23 +1351,23 @@
       <c r="I6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
     </row>
     <row r="7" spans="1:14" ht="212" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>0</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
@@ -1361,7 +1379,7 @@
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>13</v>
@@ -1372,13 +1390,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
@@ -1390,7 +1408,7 @@
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>13</v>
@@ -1401,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
@@ -1422,7 +1440,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="19"/>
@@ -1441,9 +1459,11 @@
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="12"/>
+        <v>56</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="D11" s="12"/>
       <c r="E11" s="26" t="s">
         <v>52</v>
@@ -1465,63 +1485,63 @@
         <v>5</v>
       </c>
       <c r="L11" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="M11" s="9" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="12" spans="1:14" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="32">
+      <c r="A12" s="41">
         <v>5</v>
       </c>
-      <c r="B12" s="38" t="s">
-        <v>58</v>
+      <c r="B12" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="36" t="s">
-        <v>59</v>
+      <c r="E12" s="45" t="s">
+        <v>84</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="33">
+      <c r="H12" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="46">
         <v>0.27700000000000002</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="44" t="s">
         <v>4</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="M12" s="38" t="s">
-        <v>56</v>
+      <c r="L12" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" s="43" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="32"/>
-      <c r="B13" s="38"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="36"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="35"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="44"/>
       <c r="K13" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="37"/>
-      <c r="M13" s="38"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="43"/>
     </row>
     <row r="14" spans="1:14" ht="215" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
@@ -1546,10 +1566,10 @@
         <v>8</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J14" s="30" t="s">
         <v>4</v>
@@ -1581,9 +1601,9 @@
       <c r="F15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="30" t="s">
         <v>4</v>
       </c>
@@ -1613,10 +1633,10 @@
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I16" s="27">
         <v>37.299999999999997</v>
@@ -1655,7 +1675,7 @@
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H17" s="27" t="s">
         <v>33</v>
@@ -1717,13 +1737,13 @@
         <v>39</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J19" s="30" t="s">
         <v>4</v>
@@ -1748,13 +1768,13 @@
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>44</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H20" s="27" t="s">
         <v>45</v>
@@ -1776,7 +1796,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19"/>
@@ -1788,14 +1808,16 @@
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
       <c r="L21" s="24"/>
-      <c r="M21" s="25"/>
+      <c r="M21" s="31" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" spans="1:13" s="8" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>14</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19"/>
@@ -1807,10 +1829,23 @@
       <c r="J22" s="23"/>
       <c r="K22" s="23"/>
       <c r="L22" s="24"/>
-      <c r="M22" s="25"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="5"/>
+      <c r="M22" s="31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>15</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
@@ -2489,6 +2524,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="J5:J6"/>
@@ -2500,17 +2546,6 @@
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J14" r:id="rId1" xr:uid="{209E2D3F-FBF9-4789-8467-E739B81E79FB}"/>

</xml_diff>

<commit_message>
Report _ Generation papers initial findings
</commit_message>
<xml_diff>
--- a/Papers/Papers.xlsx
+++ b/Papers/Papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation-Project\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FAC97C-9A12-4C48-82C2-47DFD554E784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA66FC46-2BC5-4C7D-AD32-406B972A80D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
   <si>
     <t>6. IIHT: Medical Report Generation with
 Image-to-Indicator Hierarchical Transformer.pdf</t>
@@ -248,51 +248,6 @@
   </si>
   <si>
     <t>template-based approach</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Problem with others</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> that if at least one organ is abnormal, the report is classified as abnormal, but it still contains more normal sentences than abnormal. As a result, existing text generation models may be overly focused on widely reported normal findings. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Their sol </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Hence, we propose an approach to generating radiology re_x0002_ports by generating pathological descriptions, i.e., descriptions of abnormal findings, and then replacing corresponding normal descriptions from the normal report template with a generated pathological description.</t>
-    </r>
   </si>
   <si>
     <t>1. Image tagger
@@ -465,6 +420,123 @@
     <t>3. Sabryyyy Oother</t>
   </si>
   <si>
+    <t>ROUGE-L
+BLEU-1</t>
+  </si>
+  <si>
+    <t>0.492
+0.513</t>
+  </si>
+  <si>
+    <t>Mimic-CXR
+IU X-Ray</t>
+  </si>
+  <si>
+    <t>BLEU-1
+Refer to figure 3 p. 6</t>
+  </si>
+  <si>
+    <t>Mimic-CXR
+Open-I</t>
+  </si>
+  <si>
+    <t>IU X-RAY
+Mimic-CXR</t>
+  </si>
+  <si>
+    <t>leu-1
+Rouge-L
+leu-1
+Rouge-L</t>
+  </si>
+  <si>
+    <t>0.775
+0.817
+0.833
+0.833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IU X-RAY
+Mimic-CXR
+</t>
+  </si>
+  <si>
+    <t>stanford</t>
+  </si>
+  <si>
+    <t>reasoning</t>
+  </si>
+  <si>
+    <t>Highly Recommneded
+Good Architecture</t>
+  </si>
+  <si>
+    <t>1. the visual extractor (Pretrianed)
+2. the encoder
+3. the decoder, where the proposed memory and the integration of the memory into Transformer are mainly performed in the decoder</t>
+  </si>
+  <si>
+    <t>generate large text but it's end to end
+Memory [Decoder larger history]</t>
+  </si>
+  <si>
+    <t>Hosy</t>
+  </si>
+  <si>
+    <t>CNN+RNN + Reniformect learning Learning</t>
+  </si>
+  <si>
+    <t>15.Clinically Accurate Chest X-Ray Report Generation.pdf</t>
+  </si>
+  <si>
+    <t>multi_model</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Problem with others</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that if at least one organ is abnormal, the report is classified as abnormal, but it still contains more normal sentences than abnormal. As a result, existing text generation models may be overly focused on widely reported normal findings. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Their sol </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hence, we propose an approach to generating radiology reports by generating pathological descriptions, i.e., descriptions of abnormal findings, and then replacing corresponding normal descriptions from the normal report template with a generated pathological description.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1.CNN Densenet-121  </t>
     </r>
@@ -488,80 +560,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2. Text Generation, we manually curated a set of two sentences per ab_x0002_normality indicating presence and absence, totaling 26 sentences</t>
+      <t>2. Text Generation, we manually curated a set of two sentences per abnormality indicating presence and absence, totaling 26 sentences</t>
     </r>
   </si>
   <si>
-    <t>ROUGE-L
-BLEU-1</t>
-  </si>
-  <si>
-    <t>0.492
-0.513</t>
-  </si>
-  <si>
-    <t>Mimic-CXR
-IU X-Ray</t>
-  </si>
-  <si>
-    <t>BLEU-1
-Refer to figure 3 p. 6</t>
-  </si>
-  <si>
-    <t>Mimic-CXR
-Open-I</t>
-  </si>
-  <si>
-    <t>IU X-RAY
-Mimic-CXR</t>
-  </si>
-  <si>
-    <t>leu-1
-Rouge-L
-leu-1
-Rouge-L</t>
-  </si>
-  <si>
-    <t>0.775
-0.817
-0.833
-0.833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IU X-RAY
-Mimic-CXR
-</t>
-  </si>
-  <si>
-    <t>stanford</t>
-  </si>
-  <si>
-    <t>reasoning</t>
-  </si>
-  <si>
-    <t>Highly Recommneded
-Good Architecture</t>
-  </si>
-  <si>
-    <t>1. the visual extractor (Pretrianed)
-2. the encoder
-3. the decoder, where the proposed memory and the integration of the memory into Transformer are mainly performed in the decoder</t>
-  </si>
-  <si>
-    <t>generate large text but it's end to end
-Memory [Decoder larger history]</t>
-  </si>
-  <si>
-    <t>Hosy</t>
-  </si>
-  <si>
-    <t>CNN+RNN + Reniformect learning Learning</t>
-  </si>
-  <si>
-    <t>15.Clinically Accurate Chest X-Ray Report Generation.pdf</t>
-  </si>
-  <si>
-    <t>multi_model</t>
+    <t>Reread to understand</t>
+  </si>
+  <si>
+    <t>Top</t>
   </si>
 </sst>
 </file>
@@ -628,7 +634,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -653,6 +659,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -772,7 +790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -885,6 +903,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -894,26 +924,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1248,8 +1275,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="61" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1270,27 +1297,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
-        <v>48</v>
+    <row r="2" spans="1:14" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="39"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>15</v>
@@ -1299,75 +1329,78 @@
         <v>38</v>
       </c>
       <c r="F3" s="37"/>
+      <c r="L3" s="48" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="D5" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
     </row>
     <row r="7" spans="1:14" ht="212" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>0</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
@@ -1379,7 +1412,7 @@
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>13</v>
@@ -1390,13 +1423,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
@@ -1408,18 +1441,18 @@
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="8" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
+      <c r="A9" s="50">
         <v>2</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>67</v>
+      <c r="B9" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
@@ -1436,11 +1469,11 @@
       <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:14" s="8" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
+      <c r="A10" s="50">
         <v>3</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>70</v>
+      <c r="B10" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="19"/>
@@ -1455,25 +1488,25 @@
       <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:14" ht="212" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7">
+      <c r="A11" s="48">
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I11" s="27">
         <v>0.39</v>
@@ -1485,66 +1518,66 @@
         <v>5</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="41">
+      <c r="A12" s="38">
         <v>5</v>
       </c>
-      <c r="B12" s="43" t="s">
-        <v>57</v>
+      <c r="B12" s="41" t="s">
+        <v>56</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="45" t="s">
-        <v>84</v>
+      <c r="E12" s="47" t="s">
+        <v>82</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="46">
+      <c r="G12" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="39">
         <v>0.27700000000000002</v>
       </c>
-      <c r="J12" s="44" t="s">
+      <c r="J12" s="46" t="s">
         <v>4</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="M12" s="43" t="s">
-        <v>55</v>
+      <c r="L12" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" s="41" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="41"/>
-      <c r="B13" s="43"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="45"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="44"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="46"/>
       <c r="K13" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="42"/>
-      <c r="M13" s="43"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="41"/>
     </row>
     <row r="14" spans="1:14" ht="215" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7">
+      <c r="A14" s="48">
         <v>6</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -1566,10 +1599,10 @@
         <v>8</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J14" s="30" t="s">
         <v>4</v>
@@ -1583,7 +1616,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7">
+      <c r="A15" s="50">
         <v>7</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -1601,9 +1634,9 @@
       <c r="F15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="30" t="s">
         <v>4</v>
       </c>
@@ -1616,7 +1649,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7">
+      <c r="A16" s="48">
         <v>8</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1633,10 +1666,10 @@
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I16" s="27">
         <v>37.299999999999997</v>
@@ -1658,7 +1691,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="233" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7">
+      <c r="A17" s="50">
         <v>9</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1675,7 +1708,7 @@
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H17" s="27" t="s">
         <v>33</v>
@@ -1717,8 +1750,8 @@
       <c r="L18" s="24"/>
       <c r="M18" s="25"/>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7">
+    <row r="19" spans="1:13" s="3" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="48">
         <v>11</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -1728,29 +1761,29 @@
         <v>38</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J19" s="30" t="s">
         <v>4</v>
       </c>
       <c r="K19" s="12"/>
       <c r="L19" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M19" s="31" t="s">
         <v>13</v>
@@ -1761,23 +1794,23 @@
         <v>12</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="16" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="F20" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="27" t="s">
         <v>44</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="30" t="s">
@@ -1785,7 +1818,7 @@
       </c>
       <c r="K20" s="12"/>
       <c r="L20" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M20" s="31" t="s">
         <v>13</v>
@@ -1796,7 +1829,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19"/>
@@ -1817,7 +1850,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19"/>
@@ -1834,17 +1867,26 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
+      <c r="A23" s="48">
         <v>15</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
@@ -2524,6 +2566,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="E12:E13"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="H12:H13"/>
@@ -2535,17 +2588,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J14" r:id="rId1" xr:uid="{209E2D3F-FBF9-4789-8467-E739B81E79FB}"/>

</xml_diff>